<commit_message>
update to IODE flags and edit title
</commit_message>
<xml_diff>
--- a/nes-lter-poc-transect-info.xlsx
+++ b/nes-lter-poc-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-poc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC2437-320B-4E24-8940-442D79B0B352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A83207-1811-49DB-A0C2-F4764FF73F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
   <si>
     <t>attributeName</t>
   </si>
@@ -313,24 +313,12 @@
     <t>microgramsPerLiter</t>
   </si>
   <si>
-    <t>Laboratory quality flag for carbon data</t>
-  </si>
-  <si>
-    <t>Laboratory quality flag for nitrogen data</t>
-  </si>
-  <si>
     <t>good</t>
   </si>
   <si>
     <t>bad</t>
   </si>
   <si>
-    <t xml:space="preserve">missing </t>
-  </si>
-  <si>
-    <t>questionable</t>
-  </si>
-  <si>
     <t>organic matter</t>
   </si>
   <si>
@@ -395,6 +383,21 @@
   </si>
   <si>
     <t>E.</t>
+  </si>
+  <si>
+    <t>quality not evaluated, not available or unknown</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>missing data</t>
+  </si>
+  <si>
+    <t>Carbon sample IODE Quality Flag primary level for carbon data</t>
+  </si>
+  <si>
+    <t>Nitrogen sample IODE Quality Flag primary level with lab flag for value below detection</t>
   </si>
 </sst>
 </file>
@@ -442,15 +445,15 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,13 +496,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -783,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,7 +863,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>59</v>
@@ -869,7 +872,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -929,17 +932,17 @@
       <c r="A10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -947,7 +950,7 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -957,21 +960,21 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>90</v>
       </c>
       <c r="C12" t="s">
@@ -981,12 +984,12 @@
         <v>93</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -1002,7 +1005,7 @@
         <v>93</v>
       </c>
       <c r="F13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -1013,8 +1016,8 @@
       <c r="A14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>119</v>
+      <c r="B14" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -1023,7 +1026,7 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1031,28 +1034,32 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="20" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+      <c r="C20" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1062,15 +1069,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1085,117 +1092,129 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>98</v>
+      <c r="C12" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1203,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1278,10 +1297,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>76</v>
@@ -1483,7 +1502,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -1491,7 +1510,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1499,7 +1518,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1507,7 +1526,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1515,7 +1534,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1523,7 +1542,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1531,7 +1550,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1539,7 +1558,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -1547,7 +1566,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1555,7 +1574,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -1563,7 +1582,7 @@
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -1571,17 +1590,17 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
output data table in chron order, use md inputs, update metadata
</commit_message>
<xml_diff>
--- a/nes-lter-poc-transect-info.xlsx
+++ b/nes-lter-poc-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-poc-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-poc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A83207-1811-49DB-A0C2-F4764FF73F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49383464-BF33-4593-A80F-6834A3470DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="127">
   <si>
     <t>attributeName</t>
   </si>
@@ -190,9 +190,6 @@
     <t>NSF</t>
   </si>
   <si>
-    <t>OCE-1655686</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>contact</t>
   </si>
   <si>
-    <t>metadataProvider</t>
-  </si>
-  <si>
     <t>Date and time in UTC when rosette bottle closed</t>
   </si>
   <si>
@@ -238,21 +232,9 @@
     <t>Depth of sample below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
-    <t>Kate</t>
-  </si>
-  <si>
-    <t>Morkeski</t>
-  </si>
-  <si>
-    <t>kmorkeski@whoi.edu</t>
-  </si>
-  <si>
     <t>PI</t>
   </si>
   <si>
-    <t>0000-0002-2903-5851</t>
-  </si>
-  <si>
     <t>Northeast U.S. Continental Shelf</t>
   </si>
   <si>
@@ -370,9 +352,6 @@
     <t>date_time_utc</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss+hh:mm</t>
-  </si>
-  <si>
     <t>CHN</t>
   </si>
   <si>
@@ -398,6 +377,39 @@
   </si>
   <si>
     <t>Nitrogen sample IODE Quality Flag primary level with lab flag for value below detection</t>
+  </si>
+  <si>
+    <t>Joanne</t>
+  </si>
+  <si>
+    <t>Koch</t>
+  </si>
+  <si>
+    <t>jkoch@whoi.edu</t>
+  </si>
+  <si>
+    <t>OCE-2322676</t>
+  </si>
+  <si>
+    <t>OCE-2322670</t>
+  </si>
+  <si>
+    <t>OCE-2322671</t>
+  </si>
+  <si>
+    <t>OCE-2322672</t>
+  </si>
+  <si>
+    <t>OCE-2322673</t>
+  </si>
+  <si>
+    <t>OCE-2322674</t>
+  </si>
+  <si>
+    <t>OCE-2322675</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
 </sst>
 </file>
@@ -428,21 +440,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF1D1C1D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -454,6 +461,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,9 +492,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -491,19 +504,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -788,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,16 +875,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -908,7 +920,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -930,19 +942,19 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -950,62 +962,62 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>84</v>
+      <c r="A11" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="10"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="8"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -1014,10 +1026,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>115</v>
+        <v>80</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -1026,7 +1038,7 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1034,32 +1046,32 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>87</v>
+      <c r="A15" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>88</v>
+      <c r="A16" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="20" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20"/>
-      <c r="C20" s="11"/>
+      <c r="C20" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1071,7 +1083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1085,131 +1097,131 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>87</v>
+      <c r="A2" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>87</v>
+      <c r="A3" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>87</v>
+      <c r="A4" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>87</v>
+      <c r="A5" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>87</v>
+      <c r="A6" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>88</v>
+      <c r="A7" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>88</v>
+      <c r="A8" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>88</v>
+      <c r="A9" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>88</v>
+      <c r="A10" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>88</v>
+      <c r="A11" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>88</v>
+      <c r="A12" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="B12">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1235,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,7 +1295,7 @@
         <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" t="s">
         <v>49</v>
@@ -1292,69 +1304,69 @@
         <v>52</v>
       </c>
       <c r="J2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="H3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="G4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>53</v>
+      <c r="J4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1377,7 +1389,7 @@
         <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
@@ -1386,21 +1398,21 @@
         <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
       </c>
       <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
         <v>56</v>
-      </c>
-      <c r="G6" t="s">
-        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>49</v>
@@ -1409,27 +1421,27 @@
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
         <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s">
-        <v>67</v>
       </c>
       <c r="H7" t="s">
         <v>49</v>
@@ -1438,27 +1450,24 @@
         <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
         <v>49</v>
@@ -1467,13 +1476,14 @@
         <v>52</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{CA295046-575D-408C-95E4-5B2B4E4C4C5B}"/>
-    <hyperlink ref="E7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{3FF58AF3-A0C8-487C-8733-D692C05E39B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1502,7 +1512,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -1510,7 +1520,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1518,7 +1528,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1526,7 +1536,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1534,7 +1544,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1542,7 +1552,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1550,7 +1560,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1558,7 +1568,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -1566,7 +1576,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1574,7 +1584,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -1582,7 +1592,7 @@
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -1590,25 +1600,25 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
handle C values below detection
</commit_message>
<xml_diff>
--- a/nes-lter-poc-transect-info.xlsx
+++ b/nes-lter-poc-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-poc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49383464-BF33-4593-A80F-6834A3470DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA0D796-5B98-4906-8995-00575B344656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="127">
   <si>
     <t>attributeName</t>
   </si>
@@ -373,9 +373,6 @@
     <t>missing data</t>
   </si>
   <si>
-    <t>Carbon sample IODE Quality Flag primary level for carbon data</t>
-  </si>
-  <si>
     <t>Nitrogen sample IODE Quality Flag primary level with lab flag for value below detection</t>
   </si>
   <si>
@@ -410,6 +407,9 @@
   </si>
   <si>
     <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
+  <si>
+    <t>Carbon sample IODE Quality Flag primary level for carbon data with lab flag for value below detection</t>
   </si>
 </sst>
 </file>
@@ -801,7 +801,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,7 +884,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1045,12 +1045,12 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
@@ -1062,7 +1062,7 @@
         <v>82</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
         <v>60</v>
@@ -1081,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1152,21 +1152,21 @@
         <v>81</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1174,10 +1174,10 @@
         <v>82</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1185,10 +1185,10 @@
         <v>82</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,10 +1196,10 @@
         <v>82</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,10 +1207,10 @@
         <v>82</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1218,9 +1218,20 @@
         <v>82</v>
       </c>
       <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1304,7 +1315,7 @@
         <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1336,7 +1347,7 @@
         <v>52</v>
       </c>
       <c r="J3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1366,7 +1377,7 @@
         <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1398,7 +1409,7 @@
         <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1421,7 +1432,7 @@
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1450,21 +1461,21 @@
         <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
         <v>116</v>
-      </c>
-      <c r="C8" t="s">
-        <v>117</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
         <v>65</v>
@@ -1476,7 +1487,7 @@
         <v>52</v>
       </c>
       <c r="J8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>